<commit_message>
Finalized the dataset. Read in the Excel rather than the CSV.
</commit_message>
<xml_diff>
--- a/analysis/input/Huizui.xlsx
+++ b/analysis/input/Huizui.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuanfang/Desktop/Spring 2019/SOC 513 Social Research Methods II/Assignments/Archaeobotanical Project/analysis/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2C2A59-533D-524B-B51C-A425394D1BBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A44A8E9-A509-4344-B0BA-466513D3CBEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15660" xr2:uid="{62770793-0544-BC4B-8C56-FC4EBBF98114}"/>
   </bookViews>
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="195">
   <si>
     <t>Field Year</t>
   </si>
@@ -439,9 +439,6 @@
     <t>Ter.6 Unit 3 D1</t>
   </si>
   <si>
-    <t>05HYHE</t>
-  </si>
-  <si>
     <t>Huizui E</t>
   </si>
   <si>
@@ -460,15 +457,9 @@
     <t>T3 F1② B1</t>
   </si>
   <si>
-    <t>06HYHE</t>
-  </si>
-  <si>
     <t>T5 F8 layer 7</t>
   </si>
   <si>
-    <t>MY</t>
-  </si>
-  <si>
     <t>Ter./Unit 4 H4</t>
   </si>
   <si>
@@ -487,9 +478,6 @@
     <t>Ash pit 1</t>
   </si>
   <si>
-    <t>Mid/L Yang</t>
-  </si>
-  <si>
     <t>ter 2 FS layer 1</t>
   </si>
   <si>
@@ -541,9 +529,6 @@
     <t>T104 H85</t>
   </si>
   <si>
-    <t>2002`</t>
-  </si>
-  <si>
     <t>290</t>
   </si>
   <si>
@@ -553,15 +538,6 @@
     <t>T4 H12</t>
   </si>
   <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t>AP</t>
-  </si>
-  <si>
-    <t>02HYHW FX 105</t>
-  </si>
-  <si>
     <t>Huizui W</t>
   </si>
   <si>
@@ -838,10 +814,16 @@
     <t>T101 H76</t>
   </si>
   <si>
-    <t>04HYHW</t>
-  </si>
-  <si>
     <t>T3H5</t>
+  </si>
+  <si>
+    <t>Majiayao</t>
+  </si>
+  <si>
+    <t>Mid/L Yangshao</t>
+  </si>
+  <si>
+    <t>Longshan</t>
   </si>
 </sst>
 </file>
@@ -1531,13 +1513,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762AF20C-08BD-3340-859A-F8E47225EB3C}">
   <dimension ref="A1:BJ127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
@@ -1559,7 +1541,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="17" customFormat="1" ht="125" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1747,7 +1729,7 @@
       </c>
     </row>
     <row r="2" spans="1:62" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19">
+      <c r="A2" s="29">
         <v>2005</v>
       </c>
       <c r="B2" s="18"/>
@@ -1846,7 +1828,7 @@
       <c r="BE2" s="24"/>
     </row>
     <row r="3" spans="1:62" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19">
+      <c r="A3" s="29">
         <v>2005</v>
       </c>
       <c r="B3" s="18"/>
@@ -1947,17 +1929,17 @@
       <c r="BE3" s="24"/>
     </row>
     <row r="4" spans="1:62" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="29">
+        <v>2005</v>
+      </c>
+      <c r="B4" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="C4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="D4" s="29" t="s">
         <v>68</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>69</v>
       </c>
       <c r="E4" s="29" t="s">
         <v>64</v>
@@ -2019,18 +2001,18 @@
       </c>
     </row>
     <row r="5" spans="1:62" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19">
+      <c r="A5" s="29">
         <v>2005</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>63</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" s="22">
         <v>2.4700000000000002</v>
@@ -2128,18 +2110,18 @@
       </c>
     </row>
     <row r="6" spans="1:62" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19">
+      <c r="A6" s="29">
         <v>2005</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>63</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F6" s="22">
         <v>11.38</v>
@@ -2168,17 +2150,14 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N6" s="27" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O6" s="27" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P6" s="27" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+      <c r="N6" s="27">
+        <v>0</v>
+      </c>
+      <c r="O6" s="27">
+        <v>0</v>
+      </c>
+      <c r="P6" s="27">
+        <v>0</v>
       </c>
       <c r="Q6" s="18"/>
       <c r="R6" s="18"/>
@@ -2221,20 +2200,20 @@
       <c r="BE6" s="18"/>
     </row>
     <row r="7" spans="1:62" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
-        <v>73</v>
+      <c r="A7" s="29">
+        <v>2006</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>75</v>
+        <v>192</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="29">
         <v>13.72</v>
@@ -2334,18 +2313,18 @@
       </c>
     </row>
     <row r="8" spans="1:62" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19">
+      <c r="A8" s="29">
         <v>2005</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>63</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="33">
@@ -2429,18 +2408,18 @@
       <c r="BE8" s="34"/>
     </row>
     <row r="9" spans="1:62" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19">
+      <c r="A9" s="29">
         <v>2005</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>63</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F9" s="22">
         <v>3.54</v>
@@ -2530,18 +2509,18 @@
       </c>
     </row>
     <row r="10" spans="1:62" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19">
+      <c r="A10" s="29">
         <v>2005</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>63</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F10" s="22">
         <v>3.89</v>
@@ -2633,18 +2612,18 @@
       <c r="BE10" s="24"/>
     </row>
     <row r="11" spans="1:62" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19">
+      <c r="A11" s="29">
         <v>2005</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>63</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F11" s="22">
         <v>5.01</v>
@@ -2738,20 +2717,20 @@
       </c>
     </row>
     <row r="12" spans="1:62" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="29">
+        <v>2005</v>
+      </c>
+      <c r="B12" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>67</v>
-      </c>
       <c r="C12" s="29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>82</v>
+        <v>193</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F12" s="29">
         <v>0.64</v>
@@ -2809,18 +2788,18 @@
       <c r="AX12" s="30"/>
     </row>
     <row r="13" spans="1:62" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="36">
+      <c r="A13" s="29">
         <v>2005</v>
       </c>
       <c r="B13" s="35"/>
       <c r="C13" s="37" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" s="39">
         <v>2.44</v>
@@ -2917,18 +2896,18 @@
       <c r="BE13" s="41"/>
     </row>
     <row r="14" spans="1:62" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="36">
+      <c r="A14" s="29">
         <v>2005</v>
       </c>
       <c r="B14" s="35"/>
       <c r="C14" s="37" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F14" s="39">
         <v>3.65</v>
@@ -2959,17 +2938,14 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N14" s="27" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O14" s="27" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P14" s="27" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+      <c r="N14" s="27">
+        <v>0</v>
+      </c>
+      <c r="O14" s="27">
+        <v>0</v>
+      </c>
+      <c r="P14" s="27">
+        <v>0</v>
       </c>
       <c r="Q14" s="41"/>
       <c r="R14" s="41"/>
@@ -3012,18 +2988,18 @@
       <c r="BE14" s="41"/>
     </row>
     <row r="15" spans="1:62" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="36">
+      <c r="A15" s="29">
         <v>2005</v>
       </c>
       <c r="B15" s="35"/>
       <c r="C15" s="37" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E15" s="38" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F15" s="39">
         <v>0.54</v>
@@ -3052,17 +3028,14 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N15" s="27" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O15" s="27" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P15" s="27" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+      <c r="N15" s="27">
+        <v>0</v>
+      </c>
+      <c r="O15" s="27">
+        <v>0</v>
+      </c>
+      <c r="P15" s="27">
+        <v>0</v>
       </c>
       <c r="Q15" s="41"/>
       <c r="R15" s="41"/>
@@ -3105,18 +3078,18 @@
       <c r="BE15" s="35"/>
     </row>
     <row r="16" spans="1:62" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="36">
+      <c r="A16" s="29">
         <v>2005</v>
       </c>
       <c r="B16" s="35"/>
       <c r="C16" s="37" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E16" s="38" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F16" s="39">
         <v>1.3</v>
@@ -3145,17 +3118,14 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N16" s="27" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O16" s="27" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P16" s="27" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+      <c r="N16" s="27">
+        <v>0</v>
+      </c>
+      <c r="O16" s="27">
+        <v>0</v>
+      </c>
+      <c r="P16" s="27">
+        <v>0</v>
       </c>
       <c r="Q16" s="41"/>
       <c r="R16" s="41"/>
@@ -3198,18 +3168,18 @@
       <c r="BE16" s="35"/>
     </row>
     <row r="17" spans="1:57" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36">
+      <c r="A17" s="29">
         <v>2005</v>
       </c>
       <c r="B17" s="35"/>
       <c r="C17" s="36" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F17" s="39">
         <v>5.14</v>
@@ -3299,20 +3269,20 @@
       <c r="BE17" s="35"/>
     </row>
     <row r="18" spans="1:57" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="36">
+      <c r="A18" s="29">
         <v>2002</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F18" s="39"/>
       <c r="G18" s="39"/>
@@ -3412,20 +3382,20 @@
       </c>
     </row>
     <row r="19" spans="1:57" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="36">
+      <c r="A19" s="29">
         <v>2002</v>
       </c>
       <c r="B19" s="43">
         <v>286</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F19" s="39"/>
       <c r="G19" s="39"/>
@@ -3519,20 +3489,20 @@
       </c>
     </row>
     <row r="20" spans="1:57" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="36">
+      <c r="A20" s="29">
         <v>2002</v>
       </c>
       <c r="B20" s="43">
         <v>356</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F20" s="39"/>
       <c r="G20" s="39"/>
@@ -3626,20 +3596,20 @@
       </c>
     </row>
     <row r="21" spans="1:57" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36">
+      <c r="A21" s="29">
         <v>2002</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F21" s="39"/>
       <c r="G21" s="39"/>
@@ -3729,20 +3699,20 @@
       </c>
     </row>
     <row r="22" spans="1:57" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="36">
+      <c r="A22" s="29">
         <v>2002</v>
       </c>
       <c r="B22" s="43" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F22" s="39"/>
       <c r="G22" s="39"/>
@@ -3836,20 +3806,20 @@
       </c>
     </row>
     <row r="23" spans="1:57" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="36">
+      <c r="A23" s="29">
         <v>2002</v>
       </c>
       <c r="B23" s="43" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F23" s="39">
         <v>0.1</v>
@@ -3945,20 +3915,20 @@
       </c>
     </row>
     <row r="24" spans="1:57" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="36">
+      <c r="A24" s="29">
         <v>2002</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F24" s="39">
         <v>0.1</v>
@@ -4060,20 +4030,20 @@
       </c>
     </row>
     <row r="25" spans="1:57" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="36" t="s">
-        <v>100</v>
+      <c r="A25" s="29">
+        <v>2002</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F25" s="39">
         <v>0.01</v>
@@ -4181,20 +4151,20 @@
       </c>
     </row>
     <row r="26" spans="1:57" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="29" t="s">
-        <v>73</v>
+      <c r="A26" s="29">
+        <v>2006</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>104</v>
+        <v>194</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="F26" s="29">
         <v>3.93</v>
@@ -4243,20 +4213,20 @@
       <c r="AX26" s="30"/>
     </row>
     <row r="27" spans="1:57" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="29" t="s">
-        <v>106</v>
+      <c r="A27" s="29">
+        <v>2002</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G27" s="29">
         <v>0.8</v>
@@ -4332,17 +4302,17 @@
       </c>
     </row>
     <row r="28" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="44">
+      <c r="A28" s="29">
         <v>2002</v>
       </c>
       <c r="B28" s="44">
         <v>184</v>
       </c>
       <c r="C28" s="45" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D28" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E28" s="46" t="s">
         <v>64</v>
@@ -4431,17 +4401,17 @@
       <c r="BE28" s="52"/>
     </row>
     <row r="29" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="44">
+      <c r="A29" s="29">
         <v>2002</v>
       </c>
       <c r="B29" s="44">
         <v>206</v>
       </c>
       <c r="C29" s="45" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D29" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E29" s="46" t="s">
         <v>64</v>
@@ -4552,17 +4522,17 @@
       </c>
     </row>
     <row r="30" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="44">
+      <c r="A30" s="29">
         <v>2002</v>
       </c>
       <c r="B30" s="44">
         <v>207</v>
       </c>
       <c r="C30" s="45" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D30" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E30" s="54" t="s">
         <v>64</v>
@@ -4661,17 +4631,17 @@
       </c>
     </row>
     <row r="31" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="44">
+      <c r="A31" s="29">
         <v>2002</v>
       </c>
       <c r="B31" s="44">
         <v>209</v>
       </c>
       <c r="C31" s="45" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D31" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E31" s="54" t="s">
         <v>64</v>
@@ -4774,17 +4744,17 @@
       </c>
     </row>
     <row r="32" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="44">
+      <c r="A32" s="29">
         <v>2002</v>
       </c>
       <c r="B32" s="44">
         <v>190</v>
       </c>
       <c r="C32" s="45" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D32" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E32" s="46" t="s">
         <v>64</v>
@@ -4885,17 +4855,17 @@
       </c>
     </row>
     <row r="33" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="44">
+      <c r="A33" s="29">
         <v>2002</v>
       </c>
       <c r="B33" s="44">
         <v>192</v>
       </c>
       <c r="C33" s="45" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D33" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E33" s="54" t="s">
         <v>64</v>
@@ -4992,24 +4962,24 @@
       <c r="BE33" s="52"/>
     </row>
     <row r="34" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="44">
+      <c r="A34" s="29">
         <v>2002</v>
       </c>
       <c r="B34" s="44">
         <v>196</v>
       </c>
       <c r="C34" s="45" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D34" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E34" s="54" t="s">
         <v>64</v>
       </c>
       <c r="F34" s="47"/>
       <c r="G34" s="48" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H34" s="49">
         <v>1</v>
@@ -5095,17 +5065,17 @@
       <c r="BE34" s="52"/>
     </row>
     <row r="35" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="44">
+      <c r="A35" s="29">
         <v>2002</v>
       </c>
       <c r="B35" s="44">
         <v>210</v>
       </c>
       <c r="C35" s="45" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D35" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E35" s="54" t="s">
         <v>64</v>
@@ -5200,24 +5170,24 @@
       </c>
     </row>
     <row r="36" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="44">
+      <c r="A36" s="29">
         <v>2002</v>
       </c>
       <c r="B36" s="44">
         <v>215</v>
       </c>
       <c r="C36" s="45" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D36" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E36" s="54" t="s">
         <v>64</v>
       </c>
       <c r="F36" s="47"/>
       <c r="G36" s="48" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H36" s="49">
         <v>6</v>
@@ -5307,17 +5277,17 @@
       </c>
     </row>
     <row r="37" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="44">
+      <c r="A37" s="29">
         <v>2002</v>
       </c>
       <c r="B37" s="44">
         <v>219</v>
       </c>
       <c r="C37" s="45" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D37" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E37" s="54" t="s">
         <v>64</v>
@@ -5416,17 +5386,17 @@
       </c>
     </row>
     <row r="38" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="44">
+      <c r="A38" s="29">
         <v>2002</v>
       </c>
       <c r="B38" s="44">
         <v>220</v>
       </c>
       <c r="C38" s="45" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D38" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E38" s="54" t="s">
         <v>64</v>
@@ -5523,17 +5493,17 @@
       <c r="BE38" s="52"/>
     </row>
     <row r="39" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="44">
+      <c r="A39" s="29">
         <v>2002</v>
       </c>
       <c r="B39" s="44">
         <v>227</v>
       </c>
       <c r="C39" s="45" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D39" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E39" s="46" t="s">
         <v>64</v>
@@ -5626,17 +5596,17 @@
       <c r="BE39" s="52"/>
     </row>
     <row r="40" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="44">
+      <c r="A40" s="29">
         <v>2002</v>
       </c>
       <c r="B40" s="44">
         <v>250</v>
       </c>
       <c r="C40" s="45" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D40" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E40" s="46" t="s">
         <v>64</v>
@@ -5741,17 +5711,17 @@
       </c>
     </row>
     <row r="41" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="44">
+      <c r="A41" s="29">
         <v>2002</v>
       </c>
       <c r="B41" s="44">
         <v>255</v>
       </c>
       <c r="C41" s="45" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D41" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E41" s="46" t="s">
         <v>64</v>
@@ -5848,20 +5818,20 @@
       </c>
     </row>
     <row r="42" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="44">
+      <c r="A42" s="29">
         <v>2000</v>
       </c>
       <c r="B42" s="44">
         <v>23</v>
       </c>
       <c r="C42" s="45" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D42" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E42" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F42" s="47"/>
       <c r="G42" s="48">
@@ -5945,20 +5915,20 @@
       <c r="BE42" s="52"/>
     </row>
     <row r="43" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="44">
+      <c r="A43" s="29">
         <v>2000</v>
       </c>
       <c r="B43" s="44">
         <v>18</v>
       </c>
       <c r="C43" s="45" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D43" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E43" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F43" s="47"/>
       <c r="G43" s="48">
@@ -6056,20 +6026,20 @@
       </c>
     </row>
     <row r="44" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="44">
+      <c r="A44" s="29">
         <v>2000</v>
       </c>
       <c r="B44" s="44">
         <v>26</v>
       </c>
       <c r="C44" s="45" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D44" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E44" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F44" s="47"/>
       <c r="G44" s="48">
@@ -6167,20 +6137,20 @@
       </c>
     </row>
     <row r="45" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="44">
+      <c r="A45" s="29">
         <v>2000</v>
       </c>
       <c r="B45" s="44">
         <v>27</v>
       </c>
       <c r="C45" s="45" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D45" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E45" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F45" s="47"/>
       <c r="G45" s="48">
@@ -6278,20 +6248,20 @@
       </c>
     </row>
     <row r="46" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="44">
+      <c r="A46" s="29">
         <v>2002</v>
       </c>
       <c r="B46" s="44">
         <v>173</v>
       </c>
       <c r="C46" s="45" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D46" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E46" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F46" s="47"/>
       <c r="G46" s="48">
@@ -6381,20 +6351,20 @@
       </c>
     </row>
     <row r="47" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="44">
+      <c r="A47" s="29">
         <v>2002</v>
       </c>
       <c r="B47" s="44">
         <v>175</v>
       </c>
       <c r="C47" s="45" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D47" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E47" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F47" s="47"/>
       <c r="G47" s="48">
@@ -6488,20 +6458,20 @@
       </c>
     </row>
     <row r="48" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="44">
+      <c r="A48" s="29">
         <v>2002</v>
       </c>
       <c r="B48" s="44">
         <v>198</v>
       </c>
       <c r="C48" s="45" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D48" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E48" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F48" s="47"/>
       <c r="G48" s="48">
@@ -6593,20 +6563,20 @@
       </c>
     </row>
     <row r="49" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="44">
+      <c r="A49" s="29">
         <v>2002</v>
       </c>
       <c r="B49" s="44">
         <v>199</v>
       </c>
       <c r="C49" s="45" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D49" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E49" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F49" s="47"/>
       <c r="G49" s="48">
@@ -6700,20 +6670,20 @@
       </c>
     </row>
     <row r="50" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="44">
+      <c r="A50" s="29">
         <v>2002</v>
       </c>
       <c r="B50" s="44">
         <v>200</v>
       </c>
       <c r="C50" s="45" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D50" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E50" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F50" s="47"/>
       <c r="G50" s="48">
@@ -6809,20 +6779,20 @@
       </c>
     </row>
     <row r="51" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="44">
+      <c r="A51" s="29">
         <v>2002</v>
       </c>
       <c r="B51" s="44">
         <v>201</v>
       </c>
       <c r="C51" s="45" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D51" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E51" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F51" s="47"/>
       <c r="G51" s="48">
@@ -6918,20 +6888,20 @@
       </c>
     </row>
     <row r="52" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="44">
+      <c r="A52" s="29">
         <v>2002</v>
       </c>
       <c r="B52" s="44">
         <v>202</v>
       </c>
       <c r="C52" s="45" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D52" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E52" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F52" s="47"/>
       <c r="G52" s="48">
@@ -7025,20 +6995,20 @@
       </c>
     </row>
     <row r="53" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="44">
+      <c r="A53" s="29">
         <v>2002</v>
       </c>
       <c r="B53" s="44">
         <v>222</v>
       </c>
       <c r="C53" s="45" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D53" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E53" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F53" s="47"/>
       <c r="G53" s="48">
@@ -7130,20 +7100,20 @@
       <c r="BE53" s="52"/>
     </row>
     <row r="54" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="44">
+      <c r="A54" s="29">
         <v>2002</v>
       </c>
       <c r="B54" s="44">
         <v>223</v>
       </c>
       <c r="C54" s="45" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D54" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E54" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F54" s="47"/>
       <c r="G54" s="48">
@@ -7231,20 +7201,20 @@
       </c>
     </row>
     <row r="55" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="44">
+      <c r="A55" s="29">
         <v>2002</v>
       </c>
       <c r="B55" s="44">
         <v>224</v>
       </c>
       <c r="C55" s="45" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D55" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E55" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F55" s="47"/>
       <c r="G55" s="48">
@@ -7342,20 +7312,20 @@
       </c>
     </row>
     <row r="56" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="44">
+      <c r="A56" s="29">
         <v>2002</v>
       </c>
       <c r="B56" s="44">
         <v>225</v>
       </c>
       <c r="C56" s="45" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D56" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E56" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F56" s="47"/>
       <c r="G56" s="48"/>
@@ -7447,20 +7417,20 @@
       </c>
     </row>
     <row r="57" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="55">
+      <c r="A57" s="29">
         <v>2002</v>
       </c>
       <c r="B57" s="55">
         <v>168</v>
       </c>
       <c r="C57" s="56" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D57" s="55" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E57" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F57" s="57"/>
       <c r="G57" s="58">
@@ -7552,20 +7522,20 @@
       </c>
     </row>
     <row r="58" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="55">
+      <c r="A58" s="29">
         <v>2002</v>
       </c>
       <c r="B58" s="55">
         <v>170</v>
       </c>
       <c r="C58" s="56" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D58" s="55" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E58" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F58" s="57"/>
       <c r="G58" s="58">
@@ -7665,20 +7635,20 @@
       <c r="BE58" s="62"/>
     </row>
     <row r="59" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="55">
+      <c r="A59" s="29">
         <v>2002</v>
       </c>
       <c r="B59" s="55">
         <v>171</v>
       </c>
       <c r="C59" s="56" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D59" s="55" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E59" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F59" s="57"/>
       <c r="G59" s="58">
@@ -7776,20 +7746,20 @@
       </c>
     </row>
     <row r="60" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="55">
+      <c r="A60" s="29">
         <v>2002</v>
       </c>
       <c r="B60" s="55">
         <v>172</v>
       </c>
       <c r="C60" s="56" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D60" s="55" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E60" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F60" s="57"/>
       <c r="G60" s="58">
@@ -7885,20 +7855,20 @@
       </c>
     </row>
     <row r="61" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="55">
+      <c r="A61" s="29">
         <v>2002</v>
       </c>
       <c r="B61" s="55">
         <v>168</v>
       </c>
       <c r="C61" s="56" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D61" s="55" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E61" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F61" s="57"/>
       <c r="G61" s="58">
@@ -7990,20 +7960,20 @@
       </c>
     </row>
     <row r="62" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="55">
+      <c r="A62" s="29">
         <v>2002</v>
       </c>
       <c r="B62" s="55">
         <v>170</v>
       </c>
       <c r="C62" s="56" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D62" s="55" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E62" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F62" s="57"/>
       <c r="G62" s="58">
@@ -8103,20 +8073,20 @@
       <c r="BE62" s="62"/>
     </row>
     <row r="63" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="55">
+      <c r="A63" s="29">
         <v>2002</v>
       </c>
       <c r="B63" s="55">
         <v>171</v>
       </c>
       <c r="C63" s="56" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D63" s="55" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E63" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F63" s="57"/>
       <c r="G63" s="58">
@@ -8214,20 +8184,20 @@
       </c>
     </row>
     <row r="64" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="55">
+      <c r="A64" s="29">
         <v>2002</v>
       </c>
       <c r="B64" s="55">
         <v>172</v>
       </c>
       <c r="C64" s="56" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D64" s="55" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E64" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F64" s="57"/>
       <c r="G64" s="58">
@@ -8323,20 +8293,20 @@
       </c>
     </row>
     <row r="65" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="44">
+      <c r="A65" s="29">
         <v>2002</v>
       </c>
       <c r="B65" s="44">
         <v>168</v>
       </c>
       <c r="C65" s="45" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D65" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E65" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F65" s="47"/>
       <c r="G65" s="48">
@@ -8426,20 +8396,20 @@
       </c>
     </row>
     <row r="66" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="44">
+      <c r="A66" s="29">
         <v>2002</v>
       </c>
       <c r="B66" s="44">
         <v>170</v>
       </c>
       <c r="C66" s="45" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D66" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E66" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F66" s="47"/>
       <c r="G66" s="48">
@@ -8537,20 +8507,20 @@
       <c r="BE66" s="52"/>
     </row>
     <row r="67" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="44">
+      <c r="A67" s="29">
         <v>2002</v>
       </c>
       <c r="B67" s="44">
         <v>171</v>
       </c>
       <c r="C67" s="45" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D67" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E67" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F67" s="47"/>
       <c r="G67" s="48">
@@ -8646,20 +8616,20 @@
       </c>
     </row>
     <row r="68" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="44">
+      <c r="A68" s="29">
         <v>2002</v>
       </c>
       <c r="B68" s="44">
         <v>172</v>
       </c>
       <c r="C68" s="45" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D68" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E68" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F68" s="47"/>
       <c r="G68" s="48">
@@ -8753,20 +8723,20 @@
       </c>
     </row>
     <row r="69" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="44">
+      <c r="A69" s="29">
         <v>2002</v>
       </c>
       <c r="B69" s="44">
         <v>263</v>
       </c>
       <c r="C69" s="45" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D69" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E69" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F69" s="47"/>
       <c r="G69" s="48">
@@ -8858,20 +8828,20 @@
       </c>
     </row>
     <row r="70" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="44">
+      <c r="A70" s="29">
         <v>2002</v>
       </c>
       <c r="B70" s="44">
         <v>75</v>
       </c>
       <c r="C70" s="45" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D70" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E70" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F70" s="47"/>
       <c r="G70" s="48">
@@ -8973,20 +8943,20 @@
       </c>
     </row>
     <row r="71" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="44">
+      <c r="A71" s="29">
         <v>2002</v>
       </c>
       <c r="B71" s="44">
         <v>134</v>
       </c>
       <c r="C71" s="45" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D71" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E71" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F71" s="47"/>
       <c r="G71" s="48">
@@ -9082,20 +9052,20 @@
       </c>
     </row>
     <row r="72" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="44">
+      <c r="A72" s="29">
         <v>2002</v>
       </c>
       <c r="B72" s="44">
         <v>156</v>
       </c>
       <c r="C72" s="45" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D72" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E72" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F72" s="47"/>
       <c r="G72" s="48">
@@ -9189,20 +9159,20 @@
       </c>
     </row>
     <row r="73" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="44">
+      <c r="A73" s="29">
         <v>2002</v>
       </c>
       <c r="B73" s="44">
         <v>158</v>
       </c>
       <c r="C73" s="45" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D73" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E73" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F73" s="47"/>
       <c r="G73" s="48">
@@ -9300,20 +9270,20 @@
       </c>
     </row>
     <row r="74" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="44">
+      <c r="A74" s="29">
         <v>2002</v>
       </c>
       <c r="B74" s="44">
         <v>296</v>
       </c>
       <c r="C74" s="45" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D74" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E74" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F74" s="47"/>
       <c r="G74" s="48">
@@ -9405,20 +9375,20 @@
       </c>
     </row>
     <row r="75" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="44">
+      <c r="A75" s="29">
         <v>2002</v>
       </c>
       <c r="B75" s="44">
         <v>297</v>
       </c>
       <c r="C75" s="45" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D75" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E75" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F75" s="47"/>
       <c r="G75" s="48">
@@ -9510,20 +9480,20 @@
       <c r="BE75" s="52"/>
     </row>
     <row r="76" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="44">
+      <c r="A76" s="29">
         <v>2002</v>
       </c>
       <c r="B76" s="44">
         <v>312</v>
       </c>
       <c r="C76" s="45" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D76" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E76" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F76" s="47"/>
       <c r="G76" s="48">
@@ -9625,20 +9595,20 @@
       </c>
     </row>
     <row r="77" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="44">
+      <c r="A77" s="29">
         <v>2002</v>
       </c>
       <c r="B77" s="44">
         <v>321</v>
       </c>
       <c r="C77" s="45" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D77" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E77" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F77" s="47"/>
       <c r="G77" s="48">
@@ -9734,20 +9704,20 @@
       </c>
     </row>
     <row r="78" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="44">
+      <c r="A78" s="29">
         <v>2002</v>
       </c>
       <c r="B78" s="64">
         <v>331</v>
       </c>
       <c r="C78" s="45" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D78" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E78" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F78" s="47"/>
       <c r="G78" s="48">
@@ -9839,20 +9809,20 @@
       <c r="BE78" s="52"/>
     </row>
     <row r="79" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="44">
+      <c r="A79" s="29">
         <v>2002</v>
       </c>
       <c r="B79" s="64">
         <v>350</v>
       </c>
       <c r="C79" s="45" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D79" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E79" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F79" s="47"/>
       <c r="G79" s="48">
@@ -9948,20 +9918,20 @@
       </c>
     </row>
     <row r="80" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="44">
+      <c r="A80" s="29">
         <v>2002</v>
       </c>
       <c r="B80" s="64">
         <v>352</v>
       </c>
       <c r="C80" s="45" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D80" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E80" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F80" s="47"/>
       <c r="G80" s="48">
@@ -10047,20 +10017,20 @@
       <c r="BE80" s="52"/>
     </row>
     <row r="81" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="44">
+      <c r="A81" s="29">
         <v>2002</v>
       </c>
       <c r="B81" s="64">
         <v>363</v>
       </c>
       <c r="C81" s="45" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D81" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E81" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F81" s="47"/>
       <c r="G81" s="48">
@@ -10148,20 +10118,20 @@
       </c>
     </row>
     <row r="82" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="44">
+      <c r="A82" s="29">
         <v>2002</v>
       </c>
       <c r="B82" s="64">
         <v>357</v>
       </c>
       <c r="C82" s="45" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D82" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E82" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F82" s="47"/>
       <c r="G82" s="48">
@@ -10259,20 +10229,20 @@
       </c>
     </row>
     <row r="83" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="55">
+      <c r="A83" s="29">
         <v>2002</v>
       </c>
       <c r="B83" s="55">
         <v>146</v>
       </c>
       <c r="C83" s="56" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D83" s="55" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E83" s="46" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="F83" s="57"/>
       <c r="G83" s="58"/>
@@ -10366,20 +10336,20 @@
       </c>
     </row>
     <row r="84" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="45">
+      <c r="A84" s="29">
         <v>2002</v>
       </c>
       <c r="B84" s="65">
         <v>320</v>
       </c>
       <c r="C84" s="45" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D84" s="64" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E84" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F84" s="47"/>
       <c r="G84" s="47"/>
@@ -10470,20 +10440,20 @@
       </c>
     </row>
     <row r="85" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="44">
+      <c r="A85" s="29">
         <v>2002</v>
       </c>
       <c r="B85" s="44">
         <v>179</v>
       </c>
       <c r="C85" s="45" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D85" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E85" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F85" s="47"/>
       <c r="G85" s="48">
@@ -10571,20 +10541,20 @@
       </c>
     </row>
     <row r="86" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="44">
+      <c r="A86" s="29">
         <v>2002</v>
       </c>
       <c r="B86" s="44">
         <v>180</v>
       </c>
       <c r="C86" s="45" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D86" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E86" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F86" s="47"/>
       <c r="G86" s="48">
@@ -10674,20 +10644,20 @@
       </c>
     </row>
     <row r="87" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="44">
+      <c r="A87" s="29">
         <v>2002</v>
       </c>
       <c r="B87" s="44">
         <v>182</v>
       </c>
       <c r="C87" s="45" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D87" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E87" s="54" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F87" s="47"/>
       <c r="G87" s="48"/>
@@ -10781,20 +10751,20 @@
       </c>
     </row>
     <row r="88" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="44">
+      <c r="A88" s="29">
         <v>2002</v>
       </c>
       <c r="B88" s="44">
         <v>183</v>
       </c>
       <c r="C88" s="45" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D88" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E88" s="54" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F88" s="47"/>
       <c r="G88" s="48">
@@ -10890,20 +10860,20 @@
       </c>
     </row>
     <row r="89" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="44">
+      <c r="A89" s="29">
         <v>2002</v>
       </c>
       <c r="B89" s="44">
         <v>187</v>
       </c>
       <c r="C89" s="45" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D89" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E89" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F89" s="47"/>
       <c r="G89" s="48">
@@ -10995,20 +10965,20 @@
       </c>
     </row>
     <row r="90" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="44">
+      <c r="A90" s="29">
         <v>2002</v>
       </c>
       <c r="B90" s="44">
         <v>191</v>
       </c>
       <c r="C90" s="45" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D90" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E90" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F90" s="47"/>
       <c r="G90" s="48">
@@ -11108,20 +11078,20 @@
       </c>
     </row>
     <row r="91" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="44">
+      <c r="A91" s="29">
         <v>2002</v>
       </c>
       <c r="B91" s="44">
         <v>193</v>
       </c>
       <c r="C91" s="45" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D91" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E91" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F91" s="47"/>
       <c r="G91" s="48">
@@ -11223,20 +11193,20 @@
       </c>
     </row>
     <row r="92" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="44">
+      <c r="A92" s="29">
         <v>2002</v>
       </c>
       <c r="B92" s="44">
         <v>194</v>
       </c>
       <c r="C92" s="45" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D92" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E92" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F92" s="47"/>
       <c r="G92" s="48">
@@ -11340,20 +11310,20 @@
       </c>
     </row>
     <row r="93" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="44">
+      <c r="A93" s="29">
         <v>2002</v>
       </c>
       <c r="B93" s="44">
         <v>212</v>
       </c>
       <c r="C93" s="45" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="D93" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E93" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F93" s="47"/>
       <c r="G93" s="48">
@@ -11447,20 +11417,20 @@
       </c>
     </row>
     <row r="94" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="44">
+      <c r="A94" s="29">
         <v>2002</v>
       </c>
       <c r="B94" s="44">
         <v>214</v>
       </c>
       <c r="C94" s="45" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D94" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E94" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F94" s="47"/>
       <c r="G94" s="48">
@@ -11552,20 +11522,20 @@
       </c>
     </row>
     <row r="95" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="44">
+      <c r="A95" s="29">
         <v>2002</v>
       </c>
       <c r="B95" s="44">
         <v>218</v>
       </c>
       <c r="C95" s="45" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D95" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E95" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F95" s="47"/>
       <c r="G95" s="48">
@@ -11659,20 +11629,20 @@
       </c>
     </row>
     <row r="96" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="44">
+      <c r="A96" s="29">
         <v>2002</v>
       </c>
       <c r="B96" s="44">
         <v>226</v>
       </c>
       <c r="C96" s="45" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D96" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E96" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F96" s="47"/>
       <c r="G96" s="48">
@@ -11772,20 +11742,20 @@
       </c>
     </row>
     <row r="97" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="44">
+      <c r="A97" s="29">
         <v>2002</v>
       </c>
       <c r="B97" s="44">
         <v>234</v>
       </c>
       <c r="C97" s="45" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D97" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E97" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F97" s="47"/>
       <c r="G97" s="48">
@@ -11879,20 +11849,20 @@
       <c r="BE97" s="52"/>
     </row>
     <row r="98" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="44">
+      <c r="A98" s="29">
         <v>2002</v>
       </c>
       <c r="B98" s="44">
         <v>236</v>
       </c>
       <c r="C98" s="45" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D98" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E98" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F98" s="47"/>
       <c r="G98" s="48">
@@ -11986,20 +11956,20 @@
       <c r="BE98" s="52"/>
     </row>
     <row r="99" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="44">
+      <c r="A99" s="29">
         <v>2002</v>
       </c>
       <c r="B99" s="44">
         <v>237</v>
       </c>
       <c r="C99" s="45" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D99" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E99" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F99" s="47"/>
       <c r="G99" s="48">
@@ -12087,20 +12057,20 @@
       <c r="BE99" s="52"/>
     </row>
     <row r="100" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="44">
+      <c r="A100" s="29">
         <v>2002</v>
       </c>
       <c r="B100" s="44">
         <v>238</v>
       </c>
       <c r="C100" s="45" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D100" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E100" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F100" s="47"/>
       <c r="G100" s="48">
@@ -12200,20 +12170,20 @@
       </c>
     </row>
     <row r="101" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="44">
+      <c r="A101" s="29">
         <v>2002</v>
       </c>
       <c r="B101" s="44">
         <v>240</v>
       </c>
       <c r="C101" s="45" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D101" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E101" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F101" s="47"/>
       <c r="G101" s="48">
@@ -12311,20 +12281,20 @@
       </c>
     </row>
     <row r="102" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="44">
+      <c r="A102" s="29">
         <v>2002</v>
       </c>
       <c r="B102" s="44">
         <v>241</v>
       </c>
       <c r="C102" s="45" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="D102" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E102" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F102" s="47"/>
       <c r="G102" s="48"/>
@@ -12410,20 +12380,20 @@
       <c r="BE102" s="52"/>
     </row>
     <row r="103" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="44">
+      <c r="A103" s="29">
         <v>2002</v>
       </c>
       <c r="B103" s="44">
         <v>247</v>
       </c>
       <c r="C103" s="45" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D103" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E103" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F103" s="47"/>
       <c r="G103" s="48">
@@ -12521,20 +12491,20 @@
       <c r="BE103" s="52"/>
     </row>
     <row r="104" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="44">
+      <c r="A104" s="29">
         <v>2002</v>
       </c>
       <c r="B104" s="44">
         <v>252</v>
       </c>
       <c r="C104" s="45" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D104" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E104" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F104" s="47"/>
       <c r="G104" s="48">
@@ -12630,20 +12600,20 @@
       </c>
     </row>
     <row r="105" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="44">
+      <c r="A105" s="29">
         <v>2002</v>
       </c>
       <c r="B105" s="44">
         <v>253</v>
       </c>
       <c r="C105" s="45" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D105" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E105" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F105" s="47"/>
       <c r="G105" s="48">
@@ -12735,20 +12705,20 @@
       </c>
     </row>
     <row r="106" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="44">
+      <c r="A106" s="29">
         <v>2002</v>
       </c>
       <c r="B106" s="44">
         <v>260</v>
       </c>
       <c r="C106" s="45" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D106" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E106" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F106" s="47"/>
       <c r="G106" s="48">
@@ -12852,20 +12822,20 @@
       </c>
     </row>
     <row r="107" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="44">
+      <c r="A107" s="29">
         <v>2002</v>
       </c>
       <c r="B107" s="44">
         <v>261</v>
       </c>
       <c r="C107" s="45" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D107" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E107" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F107" s="47"/>
       <c r="G107" s="48">
@@ -12963,20 +12933,20 @@
       </c>
     </row>
     <row r="108" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="44">
+      <c r="A108" s="29">
         <v>2002</v>
       </c>
       <c r="B108" s="44">
         <v>265</v>
       </c>
       <c r="C108" s="45" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D108" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E108" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F108" s="47"/>
       <c r="G108" s="48">
@@ -13082,20 +13052,20 @@
       </c>
     </row>
     <row r="109" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="44">
+      <c r="A109" s="29">
         <v>2002</v>
       </c>
       <c r="B109" s="44">
         <v>266</v>
       </c>
       <c r="C109" s="45" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D109" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E109" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F109" s="47"/>
       <c r="G109" s="48">
@@ -13189,20 +13159,20 @@
       </c>
     </row>
     <row r="110" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="44">
+      <c r="A110" s="29">
         <v>2002</v>
       </c>
       <c r="B110" s="44">
         <v>166</v>
       </c>
       <c r="C110" s="45" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D110" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E110" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F110" s="47"/>
       <c r="G110" s="48">
@@ -13300,20 +13270,20 @@
       </c>
     </row>
     <row r="111" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="44">
+      <c r="A111" s="29">
         <v>2002</v>
       </c>
       <c r="B111" s="44">
         <v>177</v>
       </c>
       <c r="C111" s="45" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D111" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E111" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F111" s="47"/>
       <c r="G111" s="48">
@@ -13411,20 +13381,20 @@
       </c>
     </row>
     <row r="112" spans="1:57" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="44">
+      <c r="A112" s="29">
         <v>2002</v>
       </c>
       <c r="B112" s="44">
         <v>178</v>
       </c>
       <c r="C112" s="45" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D112" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E112" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F112" s="47"/>
       <c r="G112" s="48"/>
@@ -13514,20 +13484,20 @@
       </c>
     </row>
     <row r="113" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="44">
+      <c r="A113" s="29">
         <v>2002</v>
       </c>
       <c r="B113" s="44">
         <v>186</v>
       </c>
       <c r="C113" s="45" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D113" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E113" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F113" s="47"/>
       <c r="G113" s="48">
@@ -13625,20 +13595,20 @@
       </c>
     </row>
     <row r="114" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="44">
+      <c r="A114" s="29">
         <v>2002</v>
       </c>
       <c r="B114" s="44">
         <v>188</v>
       </c>
       <c r="C114" s="45" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D114" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E114" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F114" s="47"/>
       <c r="G114" s="48">
@@ -13730,20 +13700,20 @@
       <c r="BE114" s="52"/>
     </row>
     <row r="115" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="44">
+      <c r="A115" s="29">
         <v>2002</v>
       </c>
       <c r="B115" s="44">
         <v>216</v>
       </c>
       <c r="C115" s="45" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D115" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E115" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F115" s="47"/>
       <c r="G115" s="48">
@@ -13839,20 +13809,20 @@
       </c>
     </row>
     <row r="116" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="44">
+      <c r="A116" s="29">
         <v>2002</v>
       </c>
       <c r="B116" s="44">
         <v>228</v>
       </c>
       <c r="C116" s="45" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D116" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E116" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F116" s="47"/>
       <c r="G116" s="48">
@@ -13952,20 +13922,20 @@
       </c>
     </row>
     <row r="117" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="44">
+      <c r="A117" s="29">
         <v>2002</v>
       </c>
       <c r="B117" s="44">
         <v>229</v>
       </c>
       <c r="C117" s="45" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D117" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E117" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F117" s="47"/>
       <c r="G117" s="48">
@@ -14061,20 +14031,20 @@
       </c>
     </row>
     <row r="118" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="44">
+      <c r="A118" s="29">
         <v>2002</v>
       </c>
       <c r="B118" s="44">
         <v>230</v>
       </c>
       <c r="C118" s="45" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D118" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E118" s="54" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F118" s="47"/>
       <c r="G118" s="48">
@@ -14172,20 +14142,20 @@
       </c>
     </row>
     <row r="119" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="44">
+      <c r="A119" s="29">
         <v>2002</v>
       </c>
       <c r="B119" s="44">
         <v>245</v>
       </c>
       <c r="C119" s="45" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D119" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E119" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F119" s="47"/>
       <c r="G119" s="48"/>
@@ -14269,20 +14239,20 @@
       </c>
     </row>
     <row r="120" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="44">
+      <c r="A120" s="29">
         <v>2002</v>
       </c>
       <c r="B120" s="44">
         <v>256</v>
       </c>
       <c r="C120" s="45" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D120" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E120" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F120" s="47"/>
       <c r="G120" s="48">
@@ -14372,20 +14342,20 @@
       </c>
     </row>
     <row r="121" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="44">
+      <c r="A121" s="29">
         <v>2002</v>
       </c>
       <c r="B121" s="44">
         <v>262</v>
       </c>
       <c r="C121" s="45" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="D121" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E121" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F121" s="47"/>
       <c r="G121" s="48">
@@ -14483,20 +14453,20 @@
       </c>
     </row>
     <row r="122" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="44">
+      <c r="A122" s="29">
         <v>2002</v>
       </c>
       <c r="B122" s="44">
         <v>86</v>
       </c>
       <c r="C122" s="45" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D122" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E122" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F122" s="47"/>
       <c r="G122" s="48"/>
@@ -14594,20 +14564,20 @@
       <c r="BE122" s="52"/>
     </row>
     <row r="123" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="44">
+      <c r="A123" s="29">
         <v>2002</v>
       </c>
       <c r="B123" s="44">
         <v>268</v>
       </c>
       <c r="C123" s="45" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D123" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E123" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F123" s="47"/>
       <c r="G123" s="48">
@@ -14703,20 +14673,20 @@
       </c>
     </row>
     <row r="124" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="44">
+      <c r="A124" s="29">
         <v>2002</v>
       </c>
       <c r="B124" s="44">
         <v>284</v>
       </c>
       <c r="C124" s="45" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D124" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E124" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F124" s="47"/>
       <c r="G124" s="48">
@@ -14818,20 +14788,20 @@
       </c>
     </row>
     <row r="125" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="44">
+      <c r="A125" s="29">
         <v>2002</v>
       </c>
       <c r="B125" s="64">
         <v>353</v>
       </c>
       <c r="C125" s="45" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D125" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E125" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F125" s="47"/>
       <c r="G125" s="48">
@@ -14931,20 +14901,20 @@
       </c>
     </row>
     <row r="126" spans="1:61" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="44">
+      <c r="A126" s="29">
         <v>2002</v>
       </c>
       <c r="B126" s="64">
         <v>360</v>
       </c>
       <c r="C126" s="45" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D126" s="44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E126" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F126" s="47"/>
       <c r="G126" s="48">
@@ -15042,20 +15012,20 @@
       </c>
     </row>
     <row r="127" spans="1:61" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="29" t="s">
-        <v>199</v>
+      <c r="A127" s="29">
+        <v>2004</v>
       </c>
       <c r="B127" s="29" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C127" s="29" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D127" s="29" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E127" s="29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F127" s="29">
         <v>37.32</v>

</xml_diff>